<commit_message>
filters function for Spectrums TAB
</commit_message>
<xml_diff>
--- a/data_test/df1.xlsx
+++ b/data_test/df1.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11028"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\VL251876\PycharmProjects\workspace\projects\Raman\P_23_09_DataProcesingVizualization\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/HoanLe/Documents/Python/data_test/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C35BDE62-61AC-7C45-BE11-C0ED551FBF11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="500" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,15 +20,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="7">
-  <si>
-    <t>x0_A</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="8">
   <si>
     <t>fwhm_E</t>
-  </si>
-  <si>
-    <t>wafer</t>
   </si>
   <si>
     <t>P01</t>
@@ -41,11 +36,20 @@
   <si>
     <t>P07</t>
   </si>
+  <si>
+    <t>wafer name</t>
+  </si>
+  <si>
+    <t>peak position</t>
+  </si>
+  <si>
+    <t>P01 B</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -149,9 +153,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -189,9 +193,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -226,7 +230,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -261,7 +265,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -434,34 +438,34 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:C1048576"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="1"/>
-    <col min="3" max="3" width="9.140625" style="2"/>
+    <col min="1" max="1" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.1640625" style="1"/>
+    <col min="3" max="3" width="9.1640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="B2" s="1">
         <v>403.81955766272011</v>
@@ -470,9 +474,9 @@
         <v>1.9310257777362729</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B3" s="1">
         <v>403.79012242610798</v>
@@ -481,9 +485,9 @@
         <v>1.6913297557134219</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B4" s="1">
         <v>403.83719710606312</v>
@@ -492,9 +496,9 @@
         <v>1.6313560911580089</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B5" s="1">
         <v>403.46136946775079</v>
@@ -503,9 +507,9 @@
         <v>1.7375589343449289</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B6" s="1">
         <v>403.62273145479128</v>
@@ -514,9 +518,9 @@
         <v>2.8168712466281609</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B7" s="1">
         <v>403.71915300382909</v>
@@ -525,9 +529,9 @@
         <v>2.3111539813610582</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B8" s="1">
         <v>403.68396086075398</v>
@@ -536,9 +540,9 @@
         <v>0.58932619539175946</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B9" s="1">
         <v>403.79492290708453</v>
@@ -547,9 +551,9 @@
         <v>1.96794267072482</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B10" s="1">
         <v>403.67252129070403</v>
@@ -558,9 +562,9 @@
         <v>1.5183902336356689</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B11" s="1">
         <v>403.71481796426622</v>
@@ -569,9 +573,9 @@
         <v>2.436676253131131</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B12" s="1">
         <v>403.683237528966</v>
@@ -580,9 +584,9 @@
         <v>6.3339276414764403E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B13" s="1">
         <v>403.70546979131132</v>
@@ -591,9 +595,9 @@
         <v>1.662518306310701</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B14" s="1">
         <v>403.67896224333538</v>
@@ -602,9 +606,9 @@
         <v>2.1135641746087841</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B15" s="1">
         <v>403.81955766272011</v>
@@ -613,9 +617,9 @@
         <v>1.9310257777362729</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B16" s="1">
         <v>403.79012242610798</v>
@@ -624,9 +628,9 @@
         <v>1.6913297557134219</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B17" s="1">
         <v>403.83719710606312</v>
@@ -635,9 +639,9 @@
         <v>1.6313560911580089</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B18" s="1">
         <v>403.46136946775079</v>
@@ -646,9 +650,9 @@
         <v>1.7375589343449289</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B19" s="1">
         <v>403.62273145479128</v>
@@ -657,9 +661,9 @@
         <v>2.8168712466281609</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B20" s="1">
         <v>403.71915300382909</v>
@@ -668,9 +672,9 @@
         <v>2.3111539813610582</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B21" s="1">
         <v>403.68396086075398</v>
@@ -679,9 +683,9 @@
         <v>0.58932619539175946</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B22" s="1">
         <v>403.79492290708453</v>
@@ -690,9 +694,9 @@
         <v>1.96794267072482</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B23" s="1">
         <v>403.67252129070403</v>
@@ -701,9 +705,9 @@
         <v>1.5183902336356689</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B24" s="1">
         <v>403.71481796426622</v>
@@ -712,9 +716,9 @@
         <v>2.436676253131131</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B25" s="1">
         <v>403.683237528966</v>
@@ -723,9 +727,9 @@
         <v>6.3339276414764403E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B26" s="1">
         <v>403.70546979131132</v>
@@ -734,9 +738,9 @@
         <v>1.662518306310701</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B27" s="1">
         <v>403.67896224333538</v>
@@ -745,9 +749,9 @@
         <v>2.1135641746087841</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B28" s="1">
         <v>403.81955766272011</v>
@@ -756,9 +760,9 @@
         <v>1.9310257777362729</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B29" s="1">
         <v>403.79012242610798</v>
@@ -767,9 +771,9 @@
         <v>1.6913297557134219</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B30" s="1">
         <v>403.83719710606312</v>
@@ -778,9 +782,9 @@
         <v>1.6313560911580089</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B31" s="1">
         <v>403.46136946775079</v>
@@ -789,9 +793,9 @@
         <v>1.7375589343449289</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B32" s="1">
         <v>403.62273145479128</v>
@@ -800,9 +804,9 @@
         <v>2.8168712466281609</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B33" s="1">
         <v>403.71915300382909</v>
@@ -811,9 +815,9 @@
         <v>2.3111539813610582</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B34" s="1">
         <v>403.68396086075398</v>
@@ -822,9 +826,9 @@
         <v>0.58932619539175946</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B35" s="1">
         <v>403.79492290708453</v>
@@ -833,9 +837,9 @@
         <v>1.96794267072482</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B36" s="1">
         <v>403.67252129070403</v>
@@ -844,9 +848,9 @@
         <v>1.5183902336356689</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B37" s="1">
         <v>403.71481796426622</v>
@@ -855,9 +859,9 @@
         <v>2.436676253131131</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B38" s="1">
         <v>403.683237528966</v>
@@ -866,9 +870,9 @@
         <v>6.3339276414764403E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B39" s="1">
         <v>403.70546979131132</v>
@@ -877,9 +881,9 @@
         <v>1.662518306310701</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B40" s="1">
         <v>403.67896224333538</v>
@@ -888,9 +892,9 @@
         <v>2.1135641746087841</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B41" s="1">
         <v>403.81955766272011</v>
@@ -899,9 +903,9 @@
         <v>1.9310257777362729</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B42" s="1">
         <v>403.79012242610798</v>
@@ -910,9 +914,9 @@
         <v>1.6913297557134219</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B43" s="1">
         <v>403.83719710606312</v>
@@ -921,9 +925,9 @@
         <v>1.6313560911580089</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B44" s="1">
         <v>403.46136946775079</v>
@@ -932,9 +936,9 @@
         <v>1.7375589343449289</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B45" s="1">
         <v>403.62273145479128</v>
@@ -943,9 +947,9 @@
         <v>2.8168712466281609</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B46" s="1">
         <v>403.71915300382909</v>
@@ -954,9 +958,9 @@
         <v>2.3111539813610582</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B47" s="1">
         <v>403.68396086075398</v>
@@ -965,9 +969,9 @@
         <v>0.58932619539175946</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B48" s="1">
         <v>403.79492290708453</v>
@@ -976,9 +980,9 @@
         <v>1.96794267072482</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B49" s="1">
         <v>403.67252129070403</v>
@@ -987,9 +991,9 @@
         <v>1.5183902336356689</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B50" s="1">
         <v>403.71481796426622</v>
@@ -998,9 +1002,9 @@
         <v>2.436676253131131</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B51" s="1">
         <v>403.683237528966</v>
@@ -1009,9 +1013,9 @@
         <v>6.3339276414764403E-2</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B52" s="1">
         <v>403.70546979131132</v>
@@ -1020,9 +1024,9 @@
         <v>1.662518306310701</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B53" s="1">
         <v>403.67896224333538</v>

</xml_diff>

<commit_message>
new "Visu" TAB : df filters OK
</commit_message>
<xml_diff>
--- a/data_test/df1.xlsx
+++ b/data_test/df1.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11028"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/HoanLe/Documents/Python/data_test/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\VL251876\Documents\Python\SPECTROview\data_test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C35BDE62-61AC-7C45-BE11-C0ED551FBF11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="500" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="495" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="7">
   <si>
     <t>fwhm_E</t>
   </si>
@@ -37,19 +36,16 @@
     <t>P07</t>
   </si>
   <si>
-    <t>wafer name</t>
-  </si>
-  <si>
     <t>peak position</t>
   </si>
   <si>
-    <t>P01 B</t>
+    <t>wafer</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -153,9 +149,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -193,9 +189,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -230,7 +226,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -265,7 +261,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -438,34 +434,34 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.1640625" style="1"/>
-    <col min="3" max="3" width="9.1640625" style="2"/>
+    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" style="1"/>
+    <col min="3" max="3" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>5</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>6</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="B2" s="1">
         <v>403.81955766272011</v>
@@ -474,7 +470,7 @@
         <v>1.9310257777362729</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -485,7 +481,7 @@
         <v>1.6913297557134219</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -496,7 +492,7 @@
         <v>1.6313560911580089</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -507,7 +503,7 @@
         <v>1.7375589343449289</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>1</v>
       </c>
@@ -518,7 +514,7 @@
         <v>2.8168712466281609</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>1</v>
       </c>
@@ -529,7 +525,7 @@
         <v>2.3111539813610582</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>1</v>
       </c>
@@ -540,7 +536,7 @@
         <v>0.58932619539175946</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>1</v>
       </c>
@@ -551,7 +547,7 @@
         <v>1.96794267072482</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>1</v>
       </c>
@@ -562,7 +558,7 @@
         <v>1.5183902336356689</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>1</v>
       </c>
@@ -573,7 +569,7 @@
         <v>2.436676253131131</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>1</v>
       </c>
@@ -584,7 +580,7 @@
         <v>6.3339276414764403E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>1</v>
       </c>
@@ -595,7 +591,7 @@
         <v>1.662518306310701</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>1</v>
       </c>
@@ -606,7 +602,7 @@
         <v>2.1135641746087841</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>2</v>
       </c>
@@ -617,7 +613,7 @@
         <v>1.9310257777362729</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>2</v>
       </c>
@@ -628,7 +624,7 @@
         <v>1.6913297557134219</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>2</v>
       </c>
@@ -639,7 +635,7 @@
         <v>1.6313560911580089</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>2</v>
       </c>
@@ -650,7 +646,7 @@
         <v>1.7375589343449289</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>2</v>
       </c>
@@ -661,7 +657,7 @@
         <v>2.8168712466281609</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>2</v>
       </c>
@@ -672,7 +668,7 @@
         <v>2.3111539813610582</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>2</v>
       </c>
@@ -683,7 +679,7 @@
         <v>0.58932619539175946</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>2</v>
       </c>
@@ -694,7 +690,7 @@
         <v>1.96794267072482</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>2</v>
       </c>
@@ -705,7 +701,7 @@
         <v>1.5183902336356689</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>2</v>
       </c>
@@ -716,7 +712,7 @@
         <v>2.436676253131131</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>2</v>
       </c>
@@ -727,7 +723,7 @@
         <v>6.3339276414764403E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>2</v>
       </c>
@@ -738,7 +734,7 @@
         <v>1.662518306310701</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>2</v>
       </c>
@@ -749,7 +745,7 @@
         <v>2.1135641746087841</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>3</v>
       </c>
@@ -760,7 +756,7 @@
         <v>1.9310257777362729</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>3</v>
       </c>
@@ -771,7 +767,7 @@
         <v>1.6913297557134219</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>3</v>
       </c>
@@ -782,7 +778,7 @@
         <v>1.6313560911580089</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>3</v>
       </c>
@@ -793,7 +789,7 @@
         <v>1.7375589343449289</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>3</v>
       </c>
@@ -804,7 +800,7 @@
         <v>2.8168712466281609</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>3</v>
       </c>
@@ -815,7 +811,7 @@
         <v>2.3111539813610582</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>3</v>
       </c>
@@ -826,7 +822,7 @@
         <v>0.58932619539175946</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>3</v>
       </c>
@@ -837,7 +833,7 @@
         <v>1.96794267072482</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>3</v>
       </c>
@@ -848,7 +844,7 @@
         <v>1.5183902336356689</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>3</v>
       </c>
@@ -859,7 +855,7 @@
         <v>2.436676253131131</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>3</v>
       </c>
@@ -870,7 +866,7 @@
         <v>6.3339276414764403E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>3</v>
       </c>
@@ -881,7 +877,7 @@
         <v>1.662518306310701</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>3</v>
       </c>
@@ -892,7 +888,7 @@
         <v>2.1135641746087841</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>4</v>
       </c>
@@ -903,7 +899,7 @@
         <v>1.9310257777362729</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>4</v>
       </c>
@@ -914,7 +910,7 @@
         <v>1.6913297557134219</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>4</v>
       </c>
@@ -925,7 +921,7 @@
         <v>1.6313560911580089</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>4</v>
       </c>
@@ -936,7 +932,7 @@
         <v>1.7375589343449289</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>4</v>
       </c>
@@ -947,7 +943,7 @@
         <v>2.8168712466281609</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>4</v>
       </c>
@@ -958,7 +954,7 @@
         <v>2.3111539813610582</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>4</v>
       </c>
@@ -969,7 +965,7 @@
         <v>0.58932619539175946</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>4</v>
       </c>
@@ -980,7 +976,7 @@
         <v>1.96794267072482</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>4</v>
       </c>
@@ -991,7 +987,7 @@
         <v>1.5183902336356689</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>4</v>
       </c>
@@ -1002,7 +998,7 @@
         <v>2.436676253131131</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>4</v>
       </c>
@@ -1013,7 +1009,7 @@
         <v>6.3339276414764403E-2</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>4</v>
       </c>
@@ -1024,7 +1020,7 @@
         <v>1.662518306310701</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>4</v>
       </c>

</xml_diff>

<commit_message>
NEW VISU tab OK
</commit_message>
<xml_diff>
--- a/data_test/df1.xlsx
+++ b/data_test/df1.xlsx
@@ -1,25 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11028"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\VL251876\Documents\Python\SPECTROview\data_test\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/HoanLe/SPECTROview/Python/data_test/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E20D16B-5835-CA4E-B960-CD8BAAB7290B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="495" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="8">
   <si>
     <t>fwhm_E</t>
   </si>
@@ -41,11 +55,14 @@
   <si>
     <t>wafer</t>
   </si>
+  <si>
+    <t>peak2</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -97,7 +114,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -120,15 +137,29 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -149,9 +180,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -189,9 +220,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -226,7 +257,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -261,7 +292,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -434,21 +465,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C53"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="1"/>
-    <col min="3" max="3" width="9.140625" style="2"/>
+    <col min="1" max="1" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.1640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="9.1640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>6</v>
       </c>
@@ -458,8 +489,11 @@
       <c r="C1" s="3" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -469,8 +503,12 @@
       <c r="C2" s="2">
         <v>1.9310257777362729</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2">
+        <f>B2*1.13</f>
+        <v>456.31610015887367</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -480,8 +518,12 @@
       <c r="C3" s="2">
         <v>1.6913297557134219</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3">
+        <f t="shared" ref="D3:D53" si="0">B3*1.13</f>
+        <v>456.28283834150199</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -491,8 +533,12 @@
       <c r="C4" s="2">
         <v>1.6313560911580089</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4">
+        <f t="shared" si="0"/>
+        <v>456.3360327298513</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -502,8 +548,12 @@
       <c r="C5" s="2">
         <v>1.7375589343449289</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>455.91134749855837</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>1</v>
       </c>
@@ -513,8 +563,12 @@
       <c r="C6" s="2">
         <v>2.8168712466281609</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D6">
+        <f t="shared" si="0"/>
+        <v>456.09368654391409</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>1</v>
       </c>
@@ -524,8 +578,12 @@
       <c r="C7" s="2">
         <v>2.3111539813610582</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>456.20264289432686</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>1</v>
       </c>
@@ -535,8 +593,12 @@
       <c r="C8" s="2">
         <v>0.58932619539175946</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>456.16287577265194</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>1</v>
       </c>
@@ -546,8 +608,12 @@
       <c r="C9" s="2">
         <v>1.96794267072482</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>456.28826288500545</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>1</v>
       </c>
@@ -557,8 +623,12 @@
       <c r="C10" s="2">
         <v>1.5183902336356689</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>456.14994905849551</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>1</v>
       </c>
@@ -568,8 +638,12 @@
       <c r="C11" s="2">
         <v>2.436676253131131</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D11">
+        <f t="shared" si="0"/>
+        <v>456.19774429962081</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>1</v>
       </c>
@@ -579,8 +653,12 @@
       <c r="C12" s="2">
         <v>6.3339276414764403E-2</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>456.16205840773154</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>1</v>
       </c>
@@ -590,8 +668,12 @@
       <c r="C13" s="2">
         <v>1.662518306310701</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D13">
+        <f t="shared" si="0"/>
+        <v>456.18718086418176</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>1</v>
       </c>
@@ -601,8 +683,12 @@
       <c r="C14" s="2">
         <v>2.1135641746087841</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D14">
+        <f t="shared" si="0"/>
+        <v>456.15722733496892</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>2</v>
       </c>
@@ -612,8 +698,12 @@
       <c r="C15" s="2">
         <v>1.9310257777362729</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D15">
+        <f t="shared" si="0"/>
+        <v>456.31610015887367</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>2</v>
       </c>
@@ -623,8 +713,12 @@
       <c r="C16" s="2">
         <v>1.6913297557134219</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D16">
+        <f t="shared" si="0"/>
+        <v>456.28283834150199</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>2</v>
       </c>
@@ -634,8 +728,12 @@
       <c r="C17" s="2">
         <v>1.6313560911580089</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D17">
+        <f t="shared" si="0"/>
+        <v>456.3360327298513</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>2</v>
       </c>
@@ -645,8 +743,12 @@
       <c r="C18" s="2">
         <v>1.7375589343449289</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D18">
+        <f t="shared" si="0"/>
+        <v>455.91134749855837</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>2</v>
       </c>
@@ -656,8 +758,12 @@
       <c r="C19" s="2">
         <v>2.8168712466281609</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D19">
+        <f t="shared" si="0"/>
+        <v>456.09368654391409</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>2</v>
       </c>
@@ -667,8 +773,12 @@
       <c r="C20" s="2">
         <v>2.3111539813610582</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D20">
+        <f t="shared" si="0"/>
+        <v>456.20264289432686</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>2</v>
       </c>
@@ -678,8 +788,12 @@
       <c r="C21" s="2">
         <v>0.58932619539175946</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D21">
+        <f t="shared" si="0"/>
+        <v>456.16287577265194</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>2</v>
       </c>
@@ -689,8 +803,12 @@
       <c r="C22" s="2">
         <v>1.96794267072482</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D22">
+        <f t="shared" si="0"/>
+        <v>456.28826288500545</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>2</v>
       </c>
@@ -700,8 +818,12 @@
       <c r="C23" s="2">
         <v>1.5183902336356689</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D23">
+        <f t="shared" si="0"/>
+        <v>456.14994905849551</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>2</v>
       </c>
@@ -711,8 +833,12 @@
       <c r="C24" s="2">
         <v>2.436676253131131</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D24">
+        <f t="shared" si="0"/>
+        <v>456.19774429962081</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>2</v>
       </c>
@@ -722,8 +848,12 @@
       <c r="C25" s="2">
         <v>6.3339276414764403E-2</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D25">
+        <f t="shared" si="0"/>
+        <v>456.16205840773154</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>2</v>
       </c>
@@ -733,8 +863,12 @@
       <c r="C26" s="2">
         <v>1.662518306310701</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D26">
+        <f t="shared" si="0"/>
+        <v>456.18718086418176</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>2</v>
       </c>
@@ -744,8 +878,12 @@
       <c r="C27" s="2">
         <v>2.1135641746087841</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D27">
+        <f t="shared" si="0"/>
+        <v>456.15722733496892</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>3</v>
       </c>
@@ -755,8 +893,12 @@
       <c r="C28" s="2">
         <v>1.9310257777362729</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D28">
+        <f t="shared" si="0"/>
+        <v>456.31610015887367</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>3</v>
       </c>
@@ -766,8 +908,12 @@
       <c r="C29" s="2">
         <v>1.6913297557134219</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D29">
+        <f t="shared" si="0"/>
+        <v>456.28283834150199</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>3</v>
       </c>
@@ -777,8 +923,12 @@
       <c r="C30" s="2">
         <v>1.6313560911580089</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D30">
+        <f t="shared" si="0"/>
+        <v>456.3360327298513</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>3</v>
       </c>
@@ -788,8 +938,12 @@
       <c r="C31" s="2">
         <v>1.7375589343449289</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D31">
+        <f t="shared" si="0"/>
+        <v>455.91134749855837</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>3</v>
       </c>
@@ -799,8 +953,12 @@
       <c r="C32" s="2">
         <v>2.8168712466281609</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D32">
+        <f t="shared" si="0"/>
+        <v>456.09368654391409</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>3</v>
       </c>
@@ -810,8 +968,12 @@
       <c r="C33" s="2">
         <v>2.3111539813610582</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D33">
+        <f t="shared" si="0"/>
+        <v>456.20264289432686</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>3</v>
       </c>
@@ -821,8 +983,12 @@
       <c r="C34" s="2">
         <v>0.58932619539175946</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D34">
+        <f t="shared" si="0"/>
+        <v>456.16287577265194</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>3</v>
       </c>
@@ -832,8 +998,12 @@
       <c r="C35" s="2">
         <v>1.96794267072482</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D35">
+        <f t="shared" si="0"/>
+        <v>456.28826288500545</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>3</v>
       </c>
@@ -843,8 +1013,12 @@
       <c r="C36" s="2">
         <v>1.5183902336356689</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D36">
+        <f t="shared" si="0"/>
+        <v>456.14994905849551</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>3</v>
       </c>
@@ -854,8 +1028,12 @@
       <c r="C37" s="2">
         <v>2.436676253131131</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D37">
+        <f t="shared" si="0"/>
+        <v>456.19774429962081</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>3</v>
       </c>
@@ -865,8 +1043,12 @@
       <c r="C38" s="2">
         <v>6.3339276414764403E-2</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D38">
+        <f t="shared" si="0"/>
+        <v>456.16205840773154</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>3</v>
       </c>
@@ -876,8 +1058,12 @@
       <c r="C39" s="2">
         <v>1.662518306310701</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D39">
+        <f t="shared" si="0"/>
+        <v>456.18718086418176</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>3</v>
       </c>
@@ -887,8 +1073,12 @@
       <c r="C40" s="2">
         <v>2.1135641746087841</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D40">
+        <f t="shared" si="0"/>
+        <v>456.15722733496892</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>4</v>
       </c>
@@ -898,8 +1088,12 @@
       <c r="C41" s="2">
         <v>1.9310257777362729</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D41">
+        <f t="shared" si="0"/>
+        <v>456.31610015887367</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>4</v>
       </c>
@@ -909,8 +1103,12 @@
       <c r="C42" s="2">
         <v>1.6913297557134219</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D42">
+        <f t="shared" si="0"/>
+        <v>456.28283834150199</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>4</v>
       </c>
@@ -920,8 +1118,12 @@
       <c r="C43" s="2">
         <v>1.6313560911580089</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D43">
+        <f t="shared" si="0"/>
+        <v>456.3360327298513</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>4</v>
       </c>
@@ -931,8 +1133,12 @@
       <c r="C44" s="2">
         <v>1.7375589343449289</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D44">
+        <f t="shared" si="0"/>
+        <v>455.91134749855837</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>4</v>
       </c>
@@ -942,8 +1148,12 @@
       <c r="C45" s="2">
         <v>2.8168712466281609</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D45">
+        <f t="shared" si="0"/>
+        <v>456.09368654391409</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>4</v>
       </c>
@@ -953,8 +1163,12 @@
       <c r="C46" s="2">
         <v>2.3111539813610582</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D46">
+        <f t="shared" si="0"/>
+        <v>456.20264289432686</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>4</v>
       </c>
@@ -964,8 +1178,12 @@
       <c r="C47" s="2">
         <v>0.58932619539175946</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D47">
+        <f t="shared" si="0"/>
+        <v>456.16287577265194</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>4</v>
       </c>
@@ -975,8 +1193,12 @@
       <c r="C48" s="2">
         <v>1.96794267072482</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D48">
+        <f t="shared" si="0"/>
+        <v>456.28826288500545</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>4</v>
       </c>
@@ -986,8 +1208,12 @@
       <c r="C49" s="2">
         <v>1.5183902336356689</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D49">
+        <f t="shared" si="0"/>
+        <v>456.14994905849551</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>4</v>
       </c>
@@ -997,8 +1223,12 @@
       <c r="C50" s="2">
         <v>2.436676253131131</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D50">
+        <f t="shared" si="0"/>
+        <v>456.19774429962081</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>4</v>
       </c>
@@ -1008,8 +1238,12 @@
       <c r="C51" s="2">
         <v>6.3339276414764403E-2</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D51">
+        <f t="shared" si="0"/>
+        <v>456.16205840773154</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>4</v>
       </c>
@@ -1019,8 +1253,12 @@
       <c r="C52" s="2">
         <v>1.662518306310701</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D52">
+        <f t="shared" si="0"/>
+        <v>456.18718086418176</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>4</v>
       </c>
@@ -1029,6 +1267,10 @@
       </c>
       <c r="C53" s="2">
         <v>2.1135641746087841</v>
+      </c>
+      <c r="D53">
+        <f t="shared" si="0"/>
+        <v>456.15722733496892</v>
       </c>
     </row>
   </sheetData>

</xml_diff>